<commit_message>
[lab1] almost to release
</commit_message>
<xml_diff>
--- a/lab1/whetstone_statistics.xlsx
+++ b/lab1/whetstone_statistics.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Desktop\computer_architecture_engineering\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F6F2F8-2912-4533-AD9B-1BF67124FCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0245C4E-3DCB-4083-8577-3E7357D2C167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="168" windowWidth="22128" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2088" windowWidth="17280" windowHeight="9072" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>10^6</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,6 +49,22 @@
   </si>
   <si>
     <t>10^7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -89,7 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -371,17 +391,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
@@ -443,9 +469,507 @@
       <c r="B5">
         <v>1895.6</v>
       </c>
+      <c r="C5">
+        <v>1892.1</v>
+      </c>
+      <c r="D5">
+        <v>1888.2</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1895.6</v>
+        <v>1891.964252192259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>53</v>
+      </c>
+      <c r="E14">
+        <f>GEOMEAN(B14:D14)</f>
+        <v>53.331258599846869</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>522</v>
+      </c>
+      <c r="C15">
+        <v>516</v>
+      </c>
+      <c r="D15">
+        <v>531</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E17" si="1">GEOMEAN(B15:D15)</f>
+        <v>522.96373685762558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5257</v>
+      </c>
+      <c r="C16">
+        <v>5267</v>
+      </c>
+      <c r="D16">
+        <v>5280</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>5267.9915859810526</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>52753</v>
+      </c>
+      <c r="C17">
+        <v>52851</v>
+      </c>
+      <c r="D17">
+        <v>52960</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>52854.599049779186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B9D3F7-E6F3-4187-A947-EF8BE4E64E20}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>GEOMEAN(A2:C2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">GEOMEAN(A3:C3)</f>
+        <v>22.66171556604862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>226</v>
+      </c>
+      <c r="B4">
+        <v>226</v>
+      </c>
+      <c r="C4">
+        <v>225</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>225.66617381244572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2311</v>
+      </c>
+      <c r="B5">
+        <v>2296</v>
+      </c>
+      <c r="C5">
+        <v>2302</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2302.9917533813996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>50000</v>
+      </c>
+      <c r="B8">
+        <v>50000</v>
+      </c>
+      <c r="C8">
+        <v>50000</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>43478.3</v>
+      </c>
+      <c r="B9">
+        <v>43478.3</v>
+      </c>
+      <c r="C9">
+        <v>45454.5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>44127.297589263195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>44247.8</v>
+      </c>
+      <c r="B10">
+        <v>44444.4</v>
+      </c>
+      <c r="C10">
+        <v>44444.4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>44378.769799501475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>43271.3</v>
+      </c>
+      <c r="B11">
+        <v>43554</v>
+      </c>
+      <c r="C11">
+        <v>43440.4</v>
+      </c>
+      <c r="D11">
+        <f>GEOMEAN(A11:C11)</f>
+        <v>43421.744586422552</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C8158D-9CEA-47B2-92A6-7F58368BC809}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <f>GEOMEAN(A3:C3)</f>
+        <v>29.329573668739808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>221</v>
+      </c>
+      <c r="B4">
+        <v>219</v>
+      </c>
+      <c r="C4">
+        <v>221</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D6" si="0">GEOMEAN(A4:C4)</f>
+        <v>220.33131210017584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2194</v>
+      </c>
+      <c r="B5">
+        <v>2171</v>
+      </c>
+      <c r="C5">
+        <v>2184</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2182.9796821338082</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22012</v>
+      </c>
+      <c r="B6">
+        <v>21918</v>
+      </c>
+      <c r="C6">
+        <v>21893</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>21940.940242191587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3333.3</v>
+      </c>
+      <c r="B16">
+        <v>3448.3</v>
+      </c>
+      <c r="C16">
+        <v>3448.3</v>
+      </c>
+      <c r="D16">
+        <f>GEOMEAN(A16:C16)</f>
+        <v>3409.5324555196262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4524.8999999999996</v>
+      </c>
+      <c r="B17">
+        <v>4566.2</v>
+      </c>
+      <c r="C17">
+        <v>4524.8999999999996</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D19" si="1">GEOMEAN(A17:C17)</f>
+        <v>4538.6249937205903</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4557.8999999999996</v>
+      </c>
+      <c r="B18">
+        <v>4606.2</v>
+      </c>
+      <c r="C18">
+        <v>4578.6000000000004</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>4580.8572934497279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>45423</v>
+      </c>
+      <c r="B19">
+        <v>4562.5</v>
+      </c>
+      <c r="C19">
+        <v>4567.7</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>9818.8077032579222</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FD66F5-117C-46DB-8016-41AAE01A27E1}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <f>GEOMEAN(A4:C4)</f>
+        <v>28.329441987687666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>206</v>
+      </c>
+      <c r="B5">
+        <v>197</v>
+      </c>
+      <c r="C5">
+        <v>211</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D7" si="0">GEOMEAN(A5:C5)</f>
+        <v>204.58414209934182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2121</v>
+      </c>
+      <c r="B6">
+        <v>2108</v>
+      </c>
+      <c r="C6">
+        <v>2192</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2140.0172543518124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20132</v>
+      </c>
+      <c r="B7">
+        <v>21235</v>
+      </c>
+      <c r="C7">
+        <v>22023</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>21115.687299638204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3571.4</v>
+      </c>
+      <c r="B19">
+        <v>3571.4</v>
+      </c>
+      <c r="C19">
+        <v>3448.3</v>
+      </c>
+      <c r="D19">
+        <f>GEOMEAN(A19:C19)</f>
+        <v>3529.8859766091095</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4854.3999999999996</v>
+      </c>
+      <c r="B20">
+        <v>5076.1000000000004</v>
+      </c>
+      <c r="C20">
+        <v>4739.3</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D22" si="1">GEOMEAN(A20:C20)</f>
+        <v>4887.9487418499539</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4714.8</v>
+      </c>
+      <c r="B21">
+        <v>4743.8</v>
+      </c>
+      <c r="C21">
+        <v>4562</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>4672.8478688621071</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4967.2</v>
+      </c>
+      <c r="B22">
+        <v>4709.2</v>
+      </c>
+      <c r="C22">
+        <v>4540.7</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>4735.8055686720354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>